<commit_message>
- added supplier seeding - fix sample collection delete status code
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="client" sheetId="10" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="182">
   <si>
     <t>name</t>
   </si>
@@ -428,6 +428,150 @@
   </si>
   <si>
     <t>prasant2@smartfoodsafe.com</t>
+  </si>
+  <si>
+    <t>food-safe</t>
+  </si>
+  <si>
+    <t>Prasant 3</t>
+  </si>
+  <si>
+    <t>Smart Food Safe 3</t>
+  </si>
+  <si>
+    <t>prasant3@smartfoodsafe.com</t>
+  </si>
+  <si>
+    <t>contact24Hour</t>
+  </si>
+  <si>
+    <t>logisticFirstName</t>
+  </si>
+  <si>
+    <t>logisticLastName</t>
+  </si>
+  <si>
+    <t>logisticTitle</t>
+  </si>
+  <si>
+    <t>logisticEmail</t>
+  </si>
+  <si>
+    <t>logisticPhone</t>
+  </si>
+  <si>
+    <t>qaFirstName</t>
+  </si>
+  <si>
+    <t>qaLastName</t>
+  </si>
+  <si>
+    <t>qaTitle</t>
+  </si>
+  <si>
+    <t>qaEmail</t>
+  </si>
+  <si>
+    <t>qaPhone</t>
+  </si>
+  <si>
+    <t>csFirstName</t>
+  </si>
+  <si>
+    <t>csLastName</t>
+  </si>
+  <si>
+    <t>csTitle</t>
+  </si>
+  <si>
+    <t>csEmail</t>
+  </si>
+  <si>
+    <t>csPhone</t>
+  </si>
+  <si>
+    <t>supplierNote</t>
+  </si>
+  <si>
+    <t>supp1</t>
+  </si>
+  <si>
+    <t>supp2</t>
+  </si>
+  <si>
+    <t>supp3</t>
+  </si>
+  <si>
+    <t>reg1</t>
+  </si>
+  <si>
+    <t>reg2</t>
+  </si>
+  <si>
+    <t>reg3</t>
+  </si>
+  <si>
+    <t>city1</t>
+  </si>
+  <si>
+    <t>city2</t>
+  </si>
+  <si>
+    <t>city3</t>
+  </si>
+  <si>
+    <t>state1</t>
+  </si>
+  <si>
+    <t>state2</t>
+  </si>
+  <si>
+    <t>state3</t>
+  </si>
+  <si>
+    <t>country1</t>
+  </si>
+  <si>
+    <t>country2</t>
+  </si>
+  <si>
+    <t>country3</t>
+  </si>
+  <si>
+    <t>pin1</t>
+  </si>
+  <si>
+    <t>pin2</t>
+  </si>
+  <si>
+    <t>pin3</t>
+  </si>
+  <si>
+    <t>firstName1</t>
+  </si>
+  <si>
+    <t>firstName2</t>
+  </si>
+  <si>
+    <t>firstName3</t>
+  </si>
+  <si>
+    <t>lastName1</t>
+  </si>
+  <si>
+    <t>lastName2</t>
+  </si>
+  <si>
+    <t>lastName3</t>
+  </si>
+  <si>
+    <t>supp4</t>
+  </si>
+  <si>
+    <t>supp5</t>
+  </si>
+  <si>
+    <t>supp6</t>
   </si>
 </sst>
 </file>
@@ -782,7 +926,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -912,10 +1056,49 @@
         <v>7777777777</v>
       </c>
     </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="I4" s="2">
+        <v>751002</v>
+      </c>
+      <c r="J4" s="2">
+        <v>674569856</v>
+      </c>
+      <c r="K4" s="2">
+        <v>6745689865</v>
+      </c>
+      <c r="L4" s="2">
+        <v>7777777777</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1"/>
     <hyperlink ref="C3" r:id="rId2"/>
+    <hyperlink ref="C4" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1002,7 +1185,7 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="B2" sqref="B2:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1282,8 +1465,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1370,7 +1553,7 @@
         <v>122</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>122</v>
+        <v>134</v>
       </c>
       <c r="J2" s="3" t="s">
         <v>122</v>
@@ -1417,7 +1600,7 @@
         <v>123</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>123</v>
+        <v>134</v>
       </c>
       <c r="J3" s="3" t="s">
         <v>123</v>
@@ -1464,7 +1647,7 @@
         <v>124</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>124</v>
+        <v>134</v>
       </c>
       <c r="J4" s="3" t="s">
         <v>124</v>
@@ -1511,7 +1694,7 @@
         <v>125</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>125</v>
+        <v>134</v>
       </c>
       <c r="J5" s="3" t="s">
         <v>125</v>
@@ -1558,7 +1741,7 @@
         <v>126</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>126</v>
+        <v>134</v>
       </c>
       <c r="J6" s="3" t="s">
         <v>126</v>
@@ -1605,7 +1788,7 @@
         <v>127</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>127</v>
+        <v>134</v>
       </c>
       <c r="J7" s="3" t="s">
         <v>127</v>
@@ -1640,18 +1823,14 @@
     <hyperlink ref="H5" r:id="rId10"/>
     <hyperlink ref="H6" r:id="rId11"/>
     <hyperlink ref="H7" r:id="rId12"/>
-    <hyperlink ref="I2" r:id="rId13"/>
-    <hyperlink ref="I3" r:id="rId14"/>
-    <hyperlink ref="I4" r:id="rId15"/>
-    <hyperlink ref="I5" r:id="rId16"/>
-    <hyperlink ref="I6" r:id="rId17"/>
-    <hyperlink ref="I7" r:id="rId18"/>
-    <hyperlink ref="J2" r:id="rId19"/>
-    <hyperlink ref="J3" r:id="rId20"/>
-    <hyperlink ref="J4" r:id="rId21"/>
-    <hyperlink ref="J5" r:id="rId22"/>
-    <hyperlink ref="J6" r:id="rId23"/>
-    <hyperlink ref="J7" r:id="rId24"/>
+    <hyperlink ref="I2" r:id="rId13" display="p1@operator"/>
+    <hyperlink ref="J2" r:id="rId14"/>
+    <hyperlink ref="J3" r:id="rId15"/>
+    <hyperlink ref="J4" r:id="rId16"/>
+    <hyperlink ref="J5" r:id="rId17"/>
+    <hyperlink ref="J6" r:id="rId18"/>
+    <hyperlink ref="J7" r:id="rId19"/>
+    <hyperlink ref="I3:I7" r:id="rId20" display="p1@operator"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1659,22 +1838,36 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O1"/>
+  <dimension ref="A1:AF8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:J1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -1682,10 +1875,10 @@
         <v>29</v>
       </c>
       <c r="C1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" t="s">
         <v>0</v>
-      </c>
-      <c r="D1" t="s">
-        <v>30</v>
       </c>
       <c r="E1" t="s">
         <v>17</v>
@@ -1719,6 +1912,344 @@
       </c>
       <c r="O1" t="s">
         <v>36</v>
+      </c>
+      <c r="P1" t="s">
+        <v>138</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>139</v>
+      </c>
+      <c r="R1" t="s">
+        <v>140</v>
+      </c>
+      <c r="S1" t="s">
+        <v>141</v>
+      </c>
+      <c r="T1" t="s">
+        <v>142</v>
+      </c>
+      <c r="U1" t="s">
+        <v>143</v>
+      </c>
+      <c r="V1" t="s">
+        <v>144</v>
+      </c>
+      <c r="W1" t="s">
+        <v>145</v>
+      </c>
+      <c r="X1" t="s">
+        <v>146</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>147</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>148</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>149</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>150</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>151</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>152</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>153</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" t="s">
+        <v>156</v>
+      </c>
+      <c r="D2" t="s">
+        <v>156</v>
+      </c>
+      <c r="E2">
+        <v>2222222222</v>
+      </c>
+      <c r="F2" t="s">
+        <v>159</v>
+      </c>
+      <c r="G2" t="s">
+        <v>162</v>
+      </c>
+      <c r="H2" t="s">
+        <v>165</v>
+      </c>
+      <c r="I2" t="s">
+        <v>168</v>
+      </c>
+      <c r="J2" t="s">
+        <v>171</v>
+      </c>
+      <c r="K2" t="s">
+        <v>103</v>
+      </c>
+      <c r="L2" t="s">
+        <v>174</v>
+      </c>
+      <c r="M2" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C3" t="s">
+        <v>155</v>
+      </c>
+      <c r="D3" t="s">
+        <v>155</v>
+      </c>
+      <c r="E3">
+        <v>1111111111</v>
+      </c>
+      <c r="F3" t="s">
+        <v>158</v>
+      </c>
+      <c r="G3" t="s">
+        <v>161</v>
+      </c>
+      <c r="H3" t="s">
+        <v>164</v>
+      </c>
+      <c r="I3" t="s">
+        <v>167</v>
+      </c>
+      <c r="J3" t="s">
+        <v>170</v>
+      </c>
+      <c r="K3" t="s">
+        <v>103</v>
+      </c>
+      <c r="L3" t="s">
+        <v>173</v>
+      </c>
+      <c r="M3" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C4" t="s">
+        <v>156</v>
+      </c>
+      <c r="D4" t="s">
+        <v>156</v>
+      </c>
+      <c r="E4">
+        <v>2222222222</v>
+      </c>
+      <c r="F4" t="s">
+        <v>159</v>
+      </c>
+      <c r="G4" t="s">
+        <v>162</v>
+      </c>
+      <c r="H4" t="s">
+        <v>165</v>
+      </c>
+      <c r="I4" t="s">
+        <v>168</v>
+      </c>
+      <c r="J4" t="s">
+        <v>171</v>
+      </c>
+      <c r="K4" t="s">
+        <v>103</v>
+      </c>
+      <c r="L4" t="s">
+        <v>174</v>
+      </c>
+      <c r="M4" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C5" t="s">
+        <v>157</v>
+      </c>
+      <c r="D5" t="s">
+        <v>157</v>
+      </c>
+      <c r="E5">
+        <v>3333333333</v>
+      </c>
+      <c r="F5" t="s">
+        <v>160</v>
+      </c>
+      <c r="G5" t="s">
+        <v>163</v>
+      </c>
+      <c r="H5" t="s">
+        <v>166</v>
+      </c>
+      <c r="I5" t="s">
+        <v>169</v>
+      </c>
+      <c r="J5" t="s">
+        <v>172</v>
+      </c>
+      <c r="K5" t="s">
+        <v>103</v>
+      </c>
+      <c r="L5" t="s">
+        <v>175</v>
+      </c>
+      <c r="M5" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C6" t="s">
+        <v>179</v>
+      </c>
+      <c r="D6" t="s">
+        <v>155</v>
+      </c>
+      <c r="E6">
+        <v>1111111111</v>
+      </c>
+      <c r="F6" t="s">
+        <v>158</v>
+      </c>
+      <c r="G6" t="s">
+        <v>161</v>
+      </c>
+      <c r="H6" t="s">
+        <v>164</v>
+      </c>
+      <c r="I6" t="s">
+        <v>167</v>
+      </c>
+      <c r="J6" t="s">
+        <v>170</v>
+      </c>
+      <c r="K6" t="s">
+        <v>103</v>
+      </c>
+      <c r="L6" t="s">
+        <v>173</v>
+      </c>
+      <c r="M6" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C7" t="s">
+        <v>180</v>
+      </c>
+      <c r="D7" t="s">
+        <v>156</v>
+      </c>
+      <c r="E7">
+        <v>2222222222</v>
+      </c>
+      <c r="F7" t="s">
+        <v>159</v>
+      </c>
+      <c r="G7" t="s">
+        <v>162</v>
+      </c>
+      <c r="H7" t="s">
+        <v>165</v>
+      </c>
+      <c r="I7" t="s">
+        <v>168</v>
+      </c>
+      <c r="J7" t="s">
+        <v>171</v>
+      </c>
+      <c r="K7" t="s">
+        <v>103</v>
+      </c>
+      <c r="L7" t="s">
+        <v>174</v>
+      </c>
+      <c r="M7" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C8" t="s">
+        <v>181</v>
+      </c>
+      <c r="D8" t="s">
+        <v>157</v>
+      </c>
+      <c r="E8">
+        <v>3333333333</v>
+      </c>
+      <c r="F8" t="s">
+        <v>160</v>
+      </c>
+      <c r="G8" t="s">
+        <v>163</v>
+      </c>
+      <c r="H8" t="s">
+        <v>166</v>
+      </c>
+      <c r="I8" t="s">
+        <v>169</v>
+      </c>
+      <c r="J8" t="s">
+        <v>172</v>
+      </c>
+      <c r="K8" t="s">
+        <v>103</v>
+      </c>
+      <c r="L8" t="s">
+        <v>175</v>
+      </c>
+      <c r="M8" t="s">
+        <v>178</v>
       </c>
     </row>
   </sheetData>
@@ -1772,11 +2303,13 @@
   <dimension ref="A1:S1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A2" sqref="A2:A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.85546875" customWidth="1"/>
     <col min="11" max="11" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="16.140625" bestFit="1" customWidth="1"/>

</xml_diff>